<commit_message>
Comprobación de los posibles errores de lectura
</commit_message>
<xml_diff>
--- a/src/test/resources/test1.xlsx
+++ b/src/test/resources/test1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15030" windowHeight="3420"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15030" windowHeight="4815"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,37 +31,37 @@
     <t>Colegio</t>
   </si>
   <si>
-    <t>12345678A</t>
-  </si>
-  <si>
-    <t>12345678B</t>
-  </si>
-  <si>
-    <t>12345678C</t>
-  </si>
-  <si>
-    <t>Raul</t>
-  </si>
-  <si>
-    <t>Claudia</t>
-  </si>
-  <si>
-    <t>Laura</t>
-  </si>
-  <si>
-    <t>raul@uniovi.es</t>
-  </si>
-  <si>
-    <t>claudia@uniovi.es</t>
-  </si>
-  <si>
-    <t>laura@uniovi.es</t>
-  </si>
-  <si>
-    <t>Carmen</t>
-  </si>
-  <si>
-    <t>carmen@uniovi.es</t>
+    <t>Gggg</t>
+  </si>
+  <si>
+    <t>Hhhh</t>
+  </si>
+  <si>
+    <t>Iiii</t>
+  </si>
+  <si>
+    <t>Jjjj</t>
+  </si>
+  <si>
+    <t>88888888G</t>
+  </si>
+  <si>
+    <t>131313131I</t>
+  </si>
+  <si>
+    <t>14141414J</t>
+  </si>
+  <si>
+    <t>gg@uniovi.es</t>
+  </si>
+  <si>
+    <t>hh@uniovi.es</t>
+  </si>
+  <si>
+    <t>ii@uniovi.es</t>
+  </si>
+  <si>
+    <t>jj@uniovi.es</t>
   </si>
 </sst>
 </file>
@@ -415,7 +415,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,13 +441,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -455,13 +455,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B3" s="1">
+        <v>999999999</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
@@ -469,13 +469,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1">
-        <v>123456777</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1">
         <v>3</v>
@@ -483,10 +483,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>

</xml_diff>